<commit_message>
Updating example upload files for v2.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload-delete.xlsx
+++ b/data/_orig/pmhc-upload-delete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE62D53-780A-694D-953F-01B57F7F039D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FFFB26-B3F6-C743-AC66-0F277626EEF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25720" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="1020" windowWidth="25720" windowHeight="13380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="170">
   <si>
     <t>organisation_path</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>version</t>
+  </si>
+  <si>
+    <t>continuity_of_support</t>
   </si>
 </sst>
 </file>
@@ -911,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB7F861-0340-344E-9192-92E2482088FC}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
@@ -1079,15 +1082,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,10 +1176,13 @@
         <v>43</v>
       </c>
       <c r="AC1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1258,11 +1264,14 @@
       <c r="AB2">
         <v>1</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1344,8 +1353,11 @@
       <c r="AB3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1421,8 +1433,11 @@
       <c r="AB4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>

</xml_diff>